<commit_message>
Criação do arquivo executável
</commit_message>
<xml_diff>
--- a/dist/app/data/storage.xlsx
+++ b/dist/app/data/storage.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1145,6 +1145,60 @@
         </is>
       </c>
     </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>BonusPower</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>2</v>
+      </c>
+      <c r="C27" t="n">
+        <v>760</v>
+      </c>
+      <c r="D27" t="n">
+        <v>96</v>
+      </c>
+      <c r="E27" t="n">
+        <v>100</v>
+      </c>
+      <c r="F27" t="n">
+        <v>200</v>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>win</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>SkipBoss</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>2</v>
+      </c>
+      <c r="C28" t="n">
+        <v>960</v>
+      </c>
+      <c r="D28" t="n">
+        <v>96</v>
+      </c>
+      <c r="E28" t="n">
+        <v>20</v>
+      </c>
+      <c r="F28" t="n">
+        <v>40</v>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>win</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Jogando e aplicando resultados
</commit_message>
<xml_diff>
--- a/dist/app/data/storage.xlsx
+++ b/dist/app/data/storage.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1226,6 +1226,33 @@
         </is>
       </c>
     </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>BonusPower</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>2</v>
+      </c>
+      <c r="C30" t="n">
+        <v>960</v>
+      </c>
+      <c r="D30" t="n">
+        <v>96</v>
+      </c>
+      <c r="E30" t="n">
+        <v>100</v>
+      </c>
+      <c r="F30" t="n">
+        <v>200</v>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>win</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>